<commit_message>
Coleta de dados atualizada
Duas semanas de dados coletada até o momento
</commit_message>
<xml_diff>
--- a/Consumo.xlsx
+++ b/Consumo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repositorios\ConsumoDeTinta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7169562-4E71-4E73-9C20-7B90964C89EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33455C76-0086-4FE9-8BC2-C70E11D3C465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19005" yWindow="4665" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Data</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Branco 2</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0\ &quot;mL&quot;"/>
+    <numFmt numFmtId="164" formatCode="0\ &quot;mL&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -129,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -137,29 +140,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,104 +451,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>45075.45</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="5">
         <v>0.42</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="6">
         <f>B2 * 600 / 100 *100</f>
         <v>252</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="5">
         <v>0.97</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="6">
         <f>D2 * 600 / 100 * 100</f>
         <v>582</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="6">
         <f>F2 * 600 / 100 * 100</f>
         <v>330</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="5">
         <v>0.32</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="6">
         <f>H2 * 600 / 100 * 100</f>
         <v>192</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="5">
         <v>0.93</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="6">
         <f>J2 * 600 / 100 * 100</f>
         <v>558</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="5">
         <v>0.22</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="6">
         <f>L2 * 600 / 100 * 100</f>
         <v>132</v>
       </c>
+      <c r="N2" s="6">
+        <f>C2+E2+G2+I2+K2+M2</f>
+        <v>2046</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>45083.338888888888</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="C3" s="6">
+        <f>B3 * 600 / 100 *100</f>
+        <v>227.99999999999997</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="E3" s="6">
+        <f>D3 * 600 / 100 * 100</f>
+        <v>552</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.51</v>
+      </c>
+      <c r="G3" s="6">
+        <f>F3 * 600 / 100 * 100</f>
+        <v>306</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="I3" s="6">
+        <f>H3 * 600 / 100 * 100</f>
+        <v>162</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="K3" s="6">
+        <f>J3 * 600 / 100 * 100</f>
+        <v>504</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="M3" s="6">
+        <f>L3 * 600 / 100 * 100</f>
+        <v>108</v>
+      </c>
+      <c r="N3" s="6">
+        <f>C3+E3+G3+I3+K3+M3</f>
+        <v>1860</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>